<commit_message>
Added export to pdf option
</commit_message>
<xml_diff>
--- a/tests/Feature/temp/test_user.xlsx
+++ b/tests/Feature/temp/test_user.xlsx
@@ -100,27 +100,27 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Dr. Mekhi Hammes II</t>
+          <t>Jacques Friesen</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>howell.coleman@example.net</t>
+          <t>lavern.ryan@example.com</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>2025-06-21T14:20:22.000000Z</t>
+          <t>2025-06-22T19:13:32.000000Z</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>2025-06-21T14:20:22.000000Z</t>
+          <t>2025-06-22T19:13:32.000000Z</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>2025-06-21T14:20:22.000000Z</t>
+          <t>2025-06-22T19:13:32.000000Z</t>
         </is>
       </c>
     </row>
@@ -130,27 +130,27 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Cynthia Kertzmann</t>
+          <t>Marilie Wiegand</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>royce.wiza@example.net</t>
+          <t>feest.quinten@example.net</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>2025-06-21T14:20:22.000000Z</t>
+          <t>2025-06-22T19:13:32.000000Z</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>2025-06-21T14:20:22.000000Z</t>
+          <t>2025-06-22T19:13:32.000000Z</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>2025-06-21T14:20:22.000000Z</t>
+          <t>2025-06-22T19:13:32.000000Z</t>
         </is>
       </c>
     </row>
@@ -160,27 +160,27 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Dr. Lelah O'Kon</t>
+          <t>Dr. Nia Kutch</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>queen00@example.net</t>
+          <t>amanda03@example.net</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>2025-06-21T14:20:22.000000Z</t>
+          <t>2025-06-22T19:13:32.000000Z</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>2025-06-21T14:20:22.000000Z</t>
+          <t>2025-06-22T19:13:32.000000Z</t>
         </is>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>2025-06-21T14:20:22.000000Z</t>
+          <t>2025-06-22T19:13:32.000000Z</t>
         </is>
       </c>
     </row>

</xml_diff>